<commit_message>
Se agrega funcionalidad punto y coma, el compilador ahora lo distingue como FDC
</commit_message>
<xml_diff>
--- a/Base de datos/MatrizDeTransicionesBD.xlsx
+++ b/Base de datos/MatrizDeTransicionesBD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programacion\C#\ALscript-1.0\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152ACDF-0E60-4499-8191-4FBD6B4D373A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B714D33-8672-44A0-8CCC-5A2778387CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289C3FF2-1825-47B9-A7C9-E57E135FC14E}"/>
   </bookViews>
@@ -3850,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC32ADF-F58C-48F9-A000-9C1785C8F78C}">
   <dimension ref="A1:DA243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146:XFD146"/>
+    <sheetView tabSelected="1" topLeftCell="AN109" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:XFD127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43540,7 +43540,7 @@
         <v>9</v>
       </c>
       <c r="R126" s="9" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="S126" s="9" t="s">
         <v>9</v>
@@ -43857,7 +43857,7 @@
         <v>9</v>
       </c>
       <c r="R127" s="9" t="s">
-        <v>9</v>
+        <v>151</v>
       </c>
       <c r="S127" s="9" t="s">
         <v>9</v>

</xml_diff>